<commit_message>
lots lab fixes / tweaks
</commit_message>
<xml_diff>
--- a/06-mllib/kmeans/WSSSE-versus-k.xlsx
+++ b/06-mllib/kmeans/WSSSE-versus-k.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tfox/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sujee/ElephantScale/spark-labs/06-mllib/kmeans/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,9 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sample result" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>K</t>
   </si>
@@ -36,7 +40,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -44,13 +48,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -62,13 +96,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -128,7 +172,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.0792208694501422"/>
+          <c:y val="0.0198644473238314"/>
+          <c:w val="0.873384172566664"/>
+          <c:h val="0.76568438438866"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -137,7 +191,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$4</c:f>
+              <c:f>Sheet1!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -172,7 +226,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$5:$D$13</c:f>
+              <c:f>Sheet1!$A$5:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -208,37 +262,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$13</c:f>
+              <c:f>Sheet1!$B$5:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>152564.448</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>91343.409</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70849.595</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>45599.383</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>35667.768</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>33818.0996</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>19721.458</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>16784.68888</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15694.833</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -252,11 +279,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098124096"/>
-        <c:axId val="-2098128176"/>
+        <c:axId val="2115756992"/>
+        <c:axId val="2107595744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2098124096"/>
+        <c:axId val="2115756992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -313,12 +340,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098128176"/>
+        <c:crossAx val="2107595744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2098128176"/>
+        <c:axId val="2107595744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -375,7 +402,350 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098124096"/>
+        <c:crossAx val="2115756992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'sample result'!$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>WSSSE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'sample result'!$A$5:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'sample result'!$B$5:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>152564.448</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91343.409</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70849.595</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>45599.383</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35667.768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>33818.0996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19721.458</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16784.68888</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15694.833</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2143954752"/>
+        <c:axId val="2138995600"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2143954752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2138995600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2138995600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2143954752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -464,6 +834,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -980,25 +1390,578 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1278,91 +2241,170 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:E13"/>
+  <dimension ref="A4:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D5">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>2</v>
       </c>
-      <c r="E5">
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A4:B13"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
         <v>152564.448</v>
       </c>
     </row>
-    <row r="6" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D6">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>3</v>
       </c>
-      <c r="E6">
+      <c r="B6">
         <v>91343.409</v>
       </c>
     </row>
-    <row r="7" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>4</v>
       </c>
-      <c r="E7">
+      <c r="B7">
         <v>70849.595000000001</v>
       </c>
     </row>
-    <row r="8" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D8">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>5</v>
       </c>
-      <c r="E8">
+      <c r="B8">
         <v>45599.383000000002</v>
       </c>
     </row>
-    <row r="9" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D9">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>6</v>
       </c>
-      <c r="E9">
+      <c r="B9">
         <v>35667.767999999996</v>
       </c>
     </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D10">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>7</v>
       </c>
-      <c r="E10">
+      <c r="B10">
         <v>33818.099600000001</v>
       </c>
     </row>
-    <row r="11" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D11">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>8</v>
       </c>
-      <c r="E11">
+      <c r="B11">
         <v>19721.457999999999</v>
       </c>
     </row>
-    <row r="12" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D12">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>9</v>
       </c>
-      <c r="E12">
+      <c r="B12">
         <v>16784.688880000002</v>
       </c>
     </row>
-    <row r="13" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D13">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>10</v>
       </c>
-      <c r="E13">
+      <c r="B13">
         <v>15694.833000000001</v>
       </c>
     </row>

</xml_diff>